<commit_message>
Refactored codebase and updated the Readme.md
</commit_message>
<xml_diff>
--- a/Backend/oil_production_data.xlsx
+++ b/Backend/oil_production_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1790"/>
+  <dimension ref="A1:E1881"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38029,6 +38029,1917 @@
         <v>72.95</v>
       </c>
     </row>
+    <row r="1791">
+      <c r="A1791" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:52:51.423352</t>
+        </is>
+      </c>
+      <c r="B1791" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1791" t="n">
+        <v>1022.81</v>
+      </c>
+      <c r="D1791" t="n">
+        <v>1899.52</v>
+      </c>
+      <c r="E1791" t="n">
+        <v>63.79</v>
+      </c>
+    </row>
+    <row r="1792">
+      <c r="A1792" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:52:52.841970</t>
+        </is>
+      </c>
+      <c r="B1792" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1792" t="n">
+        <v>1175.88</v>
+      </c>
+      <c r="D1792" t="n">
+        <v>2006.45</v>
+      </c>
+      <c r="E1792" t="n">
+        <v>67.75</v>
+      </c>
+    </row>
+    <row r="1793">
+      <c r="A1793" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:52:54.242446</t>
+        </is>
+      </c>
+      <c r="B1793" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1793" t="n">
+        <v>1117.47</v>
+      </c>
+      <c r="D1793" t="n">
+        <v>1802.92</v>
+      </c>
+      <c r="E1793" t="n">
+        <v>68.02</v>
+      </c>
+    </row>
+    <row r="1794">
+      <c r="A1794" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:52:55.647242</t>
+        </is>
+      </c>
+      <c r="B1794" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1794" t="n">
+        <v>1135.82</v>
+      </c>
+      <c r="D1794" t="n">
+        <v>1998.14</v>
+      </c>
+      <c r="E1794" t="n">
+        <v>88.83</v>
+      </c>
+    </row>
+    <row r="1795">
+      <c r="A1795" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:52:57.150236</t>
+        </is>
+      </c>
+      <c r="B1795" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1795" t="n">
+        <v>893.52</v>
+      </c>
+      <c r="D1795" t="n">
+        <v>1814.95</v>
+      </c>
+      <c r="E1795" t="n">
+        <v>79.75</v>
+      </c>
+    </row>
+    <row r="1796">
+      <c r="A1796" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:52:58.610428</t>
+        </is>
+      </c>
+      <c r="B1796" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1796" t="n">
+        <v>996.6799999999999</v>
+      </c>
+      <c r="D1796" t="n">
+        <v>2050.7</v>
+      </c>
+      <c r="E1796" t="n">
+        <v>75.23999999999999</v>
+      </c>
+    </row>
+    <row r="1797">
+      <c r="A1797" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:00.043453</t>
+        </is>
+      </c>
+      <c r="B1797" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1797" t="n">
+        <v>1121.86</v>
+      </c>
+      <c r="D1797" t="n">
+        <v>1821.46</v>
+      </c>
+      <c r="E1797" t="n">
+        <v>70.19</v>
+      </c>
+    </row>
+    <row r="1798">
+      <c r="A1798" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:01.410910</t>
+        </is>
+      </c>
+      <c r="B1798" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1798" t="n">
+        <v>1028.56</v>
+      </c>
+      <c r="D1798" t="n">
+        <v>1851.44</v>
+      </c>
+      <c r="E1798" t="n">
+        <v>70.76000000000001</v>
+      </c>
+    </row>
+    <row r="1799">
+      <c r="A1799" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:02.793372</t>
+        </is>
+      </c>
+      <c r="B1799" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1799" t="n">
+        <v>1168.83</v>
+      </c>
+      <c r="D1799" t="n">
+        <v>2023.72</v>
+      </c>
+      <c r="E1799" t="n">
+        <v>83.40000000000001</v>
+      </c>
+    </row>
+    <row r="1800">
+      <c r="A1800" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:04.209652</t>
+        </is>
+      </c>
+      <c r="B1800" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1800" t="n">
+        <v>1089.42</v>
+      </c>
+      <c r="D1800" t="n">
+        <v>1952.01</v>
+      </c>
+      <c r="E1800" t="n">
+        <v>87.48999999999999</v>
+      </c>
+    </row>
+    <row r="1801">
+      <c r="A1801" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:05.526232</t>
+        </is>
+      </c>
+      <c r="B1801" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1801" t="n">
+        <v>1148.86</v>
+      </c>
+      <c r="D1801" t="n">
+        <v>2059.43</v>
+      </c>
+      <c r="E1801" t="n">
+        <v>87.70999999999999</v>
+      </c>
+    </row>
+    <row r="1802">
+      <c r="A1802" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:06.874426</t>
+        </is>
+      </c>
+      <c r="B1802" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1802" t="n">
+        <v>966.5</v>
+      </c>
+      <c r="D1802" t="n">
+        <v>1835.83</v>
+      </c>
+      <c r="E1802" t="n">
+        <v>81.34999999999999</v>
+      </c>
+    </row>
+    <row r="1803">
+      <c r="A1803" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:07.991757</t>
+        </is>
+      </c>
+      <c r="B1803" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1803" t="n">
+        <v>1071.63</v>
+      </c>
+      <c r="D1803" t="n">
+        <v>1839.79</v>
+      </c>
+      <c r="E1803" t="n">
+        <v>75.08</v>
+      </c>
+    </row>
+    <row r="1804">
+      <c r="A1804" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:09.123493</t>
+        </is>
+      </c>
+      <c r="B1804" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1804" t="n">
+        <v>885.03</v>
+      </c>
+      <c r="D1804" t="n">
+        <v>1923.67</v>
+      </c>
+      <c r="E1804" t="n">
+        <v>88.29000000000001</v>
+      </c>
+    </row>
+    <row r="1805">
+      <c r="A1805" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:10.254302</t>
+        </is>
+      </c>
+      <c r="B1805" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1805" t="n">
+        <v>1083.33</v>
+      </c>
+      <c r="D1805" t="n">
+        <v>1952.36</v>
+      </c>
+      <c r="E1805" t="n">
+        <v>89.70999999999999</v>
+      </c>
+    </row>
+    <row r="1806">
+      <c r="A1806" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:11.374165</t>
+        </is>
+      </c>
+      <c r="B1806" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1806" t="n">
+        <v>1085.11</v>
+      </c>
+      <c r="D1806" t="n">
+        <v>1894</v>
+      </c>
+      <c r="E1806" t="n">
+        <v>81.37</v>
+      </c>
+    </row>
+    <row r="1807">
+      <c r="A1807" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:12.497998</t>
+        </is>
+      </c>
+      <c r="B1807" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1807" t="n">
+        <v>1132.15</v>
+      </c>
+      <c r="D1807" t="n">
+        <v>1831.71</v>
+      </c>
+      <c r="E1807" t="n">
+        <v>87.56999999999999</v>
+      </c>
+    </row>
+    <row r="1808">
+      <c r="A1808" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:13.642231</t>
+        </is>
+      </c>
+      <c r="B1808" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1808" t="n">
+        <v>1196.37</v>
+      </c>
+      <c r="D1808" t="n">
+        <v>2113.85</v>
+      </c>
+      <c r="E1808" t="n">
+        <v>80.78</v>
+      </c>
+    </row>
+    <row r="1809">
+      <c r="A1809" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:14.771415</t>
+        </is>
+      </c>
+      <c r="B1809" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1809" t="n">
+        <v>1128.77</v>
+      </c>
+      <c r="D1809" t="n">
+        <v>2066.11</v>
+      </c>
+      <c r="E1809" t="n">
+        <v>82.84999999999999</v>
+      </c>
+    </row>
+    <row r="1810">
+      <c r="A1810" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:15.899627</t>
+        </is>
+      </c>
+      <c r="B1810" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1810" t="n">
+        <v>988.7</v>
+      </c>
+      <c r="D1810" t="n">
+        <v>1826.64</v>
+      </c>
+      <c r="E1810" t="n">
+        <v>79.70999999999999</v>
+      </c>
+    </row>
+    <row r="1811">
+      <c r="A1811" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:17.025388</t>
+        </is>
+      </c>
+      <c r="B1811" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1811" t="n">
+        <v>1193.71</v>
+      </c>
+      <c r="D1811" t="n">
+        <v>1977.38</v>
+      </c>
+      <c r="E1811" t="n">
+        <v>74.31999999999999</v>
+      </c>
+    </row>
+    <row r="1812">
+      <c r="A1812" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:18.158175</t>
+        </is>
+      </c>
+      <c r="B1812" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1812" t="n">
+        <v>879.4299999999999</v>
+      </c>
+      <c r="D1812" t="n">
+        <v>1870.07</v>
+      </c>
+      <c r="E1812" t="n">
+        <v>81.8</v>
+      </c>
+    </row>
+    <row r="1813">
+      <c r="A1813" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:19.275437</t>
+        </is>
+      </c>
+      <c r="B1813" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1813" t="n">
+        <v>1064.34</v>
+      </c>
+      <c r="D1813" t="n">
+        <v>2042.21</v>
+      </c>
+      <c r="E1813" t="n">
+        <v>77.83</v>
+      </c>
+    </row>
+    <row r="1814">
+      <c r="A1814" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:20.397658</t>
+        </is>
+      </c>
+      <c r="B1814" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1814" t="n">
+        <v>1199.07</v>
+      </c>
+      <c r="D1814" t="n">
+        <v>1911.2</v>
+      </c>
+      <c r="E1814" t="n">
+        <v>80.95999999999999</v>
+      </c>
+    </row>
+    <row r="1815">
+      <c r="A1815" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:21.609065</t>
+        </is>
+      </c>
+      <c r="B1815" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1815" t="n">
+        <v>833.24</v>
+      </c>
+      <c r="D1815" t="n">
+        <v>2045.23</v>
+      </c>
+      <c r="E1815" t="n">
+        <v>73.83</v>
+      </c>
+    </row>
+    <row r="1816">
+      <c r="A1816" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:22.791500</t>
+        </is>
+      </c>
+      <c r="B1816" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1816" t="n">
+        <v>1085.85</v>
+      </c>
+      <c r="D1816" t="n">
+        <v>2094.64</v>
+      </c>
+      <c r="E1816" t="n">
+        <v>82.73</v>
+      </c>
+    </row>
+    <row r="1817">
+      <c r="A1817" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:23.975289</t>
+        </is>
+      </c>
+      <c r="B1817" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1817" t="n">
+        <v>1002.34</v>
+      </c>
+      <c r="D1817" t="n">
+        <v>1858.95</v>
+      </c>
+      <c r="E1817" t="n">
+        <v>69.97</v>
+      </c>
+    </row>
+    <row r="1818">
+      <c r="A1818" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:25.188857</t>
+        </is>
+      </c>
+      <c r="B1818" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1818" t="n">
+        <v>1173.24</v>
+      </c>
+      <c r="D1818" t="n">
+        <v>1950.89</v>
+      </c>
+      <c r="E1818" t="n">
+        <v>70.34</v>
+      </c>
+    </row>
+    <row r="1819">
+      <c r="A1819" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:26.578148</t>
+        </is>
+      </c>
+      <c r="B1819" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1819" t="n">
+        <v>923.74</v>
+      </c>
+      <c r="D1819" t="n">
+        <v>1854.53</v>
+      </c>
+      <c r="E1819" t="n">
+        <v>87.20999999999999</v>
+      </c>
+    </row>
+    <row r="1820">
+      <c r="A1820" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:27.958375</t>
+        </is>
+      </c>
+      <c r="B1820" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1820" t="n">
+        <v>1095.42</v>
+      </c>
+      <c r="D1820" t="n">
+        <v>2145.65</v>
+      </c>
+      <c r="E1820" t="n">
+        <v>79.95</v>
+      </c>
+    </row>
+    <row r="1821">
+      <c r="A1821" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:29.371799</t>
+        </is>
+      </c>
+      <c r="B1821" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1821" t="n">
+        <v>1083.8</v>
+      </c>
+      <c r="D1821" t="n">
+        <v>1804.25</v>
+      </c>
+      <c r="E1821" t="n">
+        <v>68.25</v>
+      </c>
+    </row>
+    <row r="1822">
+      <c r="A1822" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:30.809843</t>
+        </is>
+      </c>
+      <c r="B1822" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1822" t="n">
+        <v>935.24</v>
+      </c>
+      <c r="D1822" t="n">
+        <v>2182.92</v>
+      </c>
+      <c r="E1822" t="n">
+        <v>71.65000000000001</v>
+      </c>
+    </row>
+    <row r="1823">
+      <c r="A1823" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:32.166938</t>
+        </is>
+      </c>
+      <c r="B1823" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1823" t="n">
+        <v>928.83</v>
+      </c>
+      <c r="D1823" t="n">
+        <v>1985.33</v>
+      </c>
+      <c r="E1823" t="n">
+        <v>73.40000000000001</v>
+      </c>
+    </row>
+    <row r="1824">
+      <c r="A1824" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:33.530731</t>
+        </is>
+      </c>
+      <c r="B1824" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1824" t="n">
+        <v>1117.48</v>
+      </c>
+      <c r="D1824" t="n">
+        <v>2052.36</v>
+      </c>
+      <c r="E1824" t="n">
+        <v>77.84999999999999</v>
+      </c>
+    </row>
+    <row r="1825">
+      <c r="A1825" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:34.880605</t>
+        </is>
+      </c>
+      <c r="B1825" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1825" t="n">
+        <v>985.27</v>
+      </c>
+      <c r="D1825" t="n">
+        <v>1961.33</v>
+      </c>
+      <c r="E1825" t="n">
+        <v>71.67</v>
+      </c>
+    </row>
+    <row r="1826">
+      <c r="A1826" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:36.294071</t>
+        </is>
+      </c>
+      <c r="B1826" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1826" t="n">
+        <v>946.74</v>
+      </c>
+      <c r="D1826" t="n">
+        <v>1977.42</v>
+      </c>
+      <c r="E1826" t="n">
+        <v>78.02</v>
+      </c>
+    </row>
+    <row r="1827">
+      <c r="A1827" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:37.729121</t>
+        </is>
+      </c>
+      <c r="B1827" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1827" t="n">
+        <v>859.24</v>
+      </c>
+      <c r="D1827" t="n">
+        <v>1993.89</v>
+      </c>
+      <c r="E1827" t="n">
+        <v>61.96</v>
+      </c>
+    </row>
+    <row r="1828">
+      <c r="A1828" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:39.273641</t>
+        </is>
+      </c>
+      <c r="B1828" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1828" t="n">
+        <v>1093.55</v>
+      </c>
+      <c r="D1828" t="n">
+        <v>2192.23</v>
+      </c>
+      <c r="E1828" t="n">
+        <v>77.43000000000001</v>
+      </c>
+    </row>
+    <row r="1829">
+      <c r="A1829" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:40.693696</t>
+        </is>
+      </c>
+      <c r="B1829" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1829" t="n">
+        <v>1069.49</v>
+      </c>
+      <c r="D1829" t="n">
+        <v>1998.51</v>
+      </c>
+      <c r="E1829" t="n">
+        <v>75.31</v>
+      </c>
+    </row>
+    <row r="1830">
+      <c r="A1830" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:42.117367</t>
+        </is>
+      </c>
+      <c r="B1830" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1830" t="n">
+        <v>948.9299999999999</v>
+      </c>
+      <c r="D1830" t="n">
+        <v>2176.11</v>
+      </c>
+      <c r="E1830" t="n">
+        <v>87.13</v>
+      </c>
+    </row>
+    <row r="1831">
+      <c r="A1831" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:43.516374</t>
+        </is>
+      </c>
+      <c r="B1831" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1831" t="n">
+        <v>945.97</v>
+      </c>
+      <c r="D1831" t="n">
+        <v>1903.38</v>
+      </c>
+      <c r="E1831" t="n">
+        <v>84.51000000000001</v>
+      </c>
+    </row>
+    <row r="1832">
+      <c r="A1832" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:45.006841</t>
+        </is>
+      </c>
+      <c r="B1832" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1832" t="n">
+        <v>973.38</v>
+      </c>
+      <c r="D1832" t="n">
+        <v>2039.29</v>
+      </c>
+      <c r="E1832" t="n">
+        <v>84.54000000000001</v>
+      </c>
+    </row>
+    <row r="1833">
+      <c r="A1833" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:46.420968</t>
+        </is>
+      </c>
+      <c r="B1833" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1833" t="n">
+        <v>1129.31</v>
+      </c>
+      <c r="D1833" t="n">
+        <v>1858.4</v>
+      </c>
+      <c r="E1833" t="n">
+        <v>67.61</v>
+      </c>
+    </row>
+    <row r="1834">
+      <c r="A1834" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:47.896775</t>
+        </is>
+      </c>
+      <c r="B1834" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1834" t="n">
+        <v>1139.33</v>
+      </c>
+      <c r="D1834" t="n">
+        <v>1801.22</v>
+      </c>
+      <c r="E1834" t="n">
+        <v>82.31999999999999</v>
+      </c>
+    </row>
+    <row r="1835">
+      <c r="A1835" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:49.322861</t>
+        </is>
+      </c>
+      <c r="B1835" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1835" t="n">
+        <v>939.5</v>
+      </c>
+      <c r="D1835" t="n">
+        <v>1919.77</v>
+      </c>
+      <c r="E1835" t="n">
+        <v>88.29000000000001</v>
+      </c>
+    </row>
+    <row r="1836">
+      <c r="A1836" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:50.783350</t>
+        </is>
+      </c>
+      <c r="B1836" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1836" t="n">
+        <v>932.1799999999999</v>
+      </c>
+      <c r="D1836" t="n">
+        <v>1860.05</v>
+      </c>
+      <c r="E1836" t="n">
+        <v>62.14</v>
+      </c>
+    </row>
+    <row r="1837">
+      <c r="A1837" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:52.213700</t>
+        </is>
+      </c>
+      <c r="B1837" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1837" t="n">
+        <v>1095.18</v>
+      </c>
+      <c r="D1837" t="n">
+        <v>1912.04</v>
+      </c>
+      <c r="E1837" t="n">
+        <v>68.98999999999999</v>
+      </c>
+    </row>
+    <row r="1838">
+      <c r="A1838" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:53.716162</t>
+        </is>
+      </c>
+      <c r="B1838" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1838" t="n">
+        <v>1007.87</v>
+      </c>
+      <c r="D1838" t="n">
+        <v>2148.08</v>
+      </c>
+      <c r="E1838" t="n">
+        <v>69.20999999999999</v>
+      </c>
+    </row>
+    <row r="1839">
+      <c r="A1839" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:55.133562</t>
+        </is>
+      </c>
+      <c r="B1839" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1839" t="n">
+        <v>987.85</v>
+      </c>
+      <c r="D1839" t="n">
+        <v>2014.2</v>
+      </c>
+      <c r="E1839" t="n">
+        <v>82.48999999999999</v>
+      </c>
+    </row>
+    <row r="1840">
+      <c r="A1840" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:56.548655</t>
+        </is>
+      </c>
+      <c r="B1840" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1840" t="n">
+        <v>861.55</v>
+      </c>
+      <c r="D1840" t="n">
+        <v>1819.98</v>
+      </c>
+      <c r="E1840" t="n">
+        <v>75.61</v>
+      </c>
+    </row>
+    <row r="1841">
+      <c r="A1841" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:57.897559</t>
+        </is>
+      </c>
+      <c r="B1841" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1841" t="n">
+        <v>980.49</v>
+      </c>
+      <c r="D1841" t="n">
+        <v>1923.59</v>
+      </c>
+      <c r="E1841" t="n">
+        <v>65.40000000000001</v>
+      </c>
+    </row>
+    <row r="1842">
+      <c r="A1842" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:53:59.292326</t>
+        </is>
+      </c>
+      <c r="B1842" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1842" t="n">
+        <v>1004.4</v>
+      </c>
+      <c r="D1842" t="n">
+        <v>1810.22</v>
+      </c>
+      <c r="E1842" t="n">
+        <v>83.19</v>
+      </c>
+    </row>
+    <row r="1843">
+      <c r="A1843" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:00.799441</t>
+        </is>
+      </c>
+      <c r="B1843" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1843" t="n">
+        <v>1016.68</v>
+      </c>
+      <c r="D1843" t="n">
+        <v>2047.05</v>
+      </c>
+      <c r="E1843" t="n">
+        <v>66.92</v>
+      </c>
+    </row>
+    <row r="1844">
+      <c r="A1844" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:02.148436</t>
+        </is>
+      </c>
+      <c r="B1844" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1844" t="n">
+        <v>940.01</v>
+      </c>
+      <c r="D1844" t="n">
+        <v>2193.69</v>
+      </c>
+      <c r="E1844" t="n">
+        <v>70.45</v>
+      </c>
+    </row>
+    <row r="1845">
+      <c r="A1845" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:03.579001</t>
+        </is>
+      </c>
+      <c r="B1845" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1845" t="n">
+        <v>913.4400000000001</v>
+      </c>
+      <c r="D1845" t="n">
+        <v>2019.71</v>
+      </c>
+      <c r="E1845" t="n">
+        <v>62.58</v>
+      </c>
+    </row>
+    <row r="1846">
+      <c r="A1846" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:05.037910</t>
+        </is>
+      </c>
+      <c r="B1846" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1846" t="n">
+        <v>861.91</v>
+      </c>
+      <c r="D1846" t="n">
+        <v>2169.05</v>
+      </c>
+      <c r="E1846" t="n">
+        <v>85.90000000000001</v>
+      </c>
+    </row>
+    <row r="1847">
+      <c r="A1847" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:06.419666</t>
+        </is>
+      </c>
+      <c r="B1847" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1847" t="n">
+        <v>939.51</v>
+      </c>
+      <c r="D1847" t="n">
+        <v>1892.55</v>
+      </c>
+      <c r="E1847" t="n">
+        <v>76.31999999999999</v>
+      </c>
+    </row>
+    <row r="1848">
+      <c r="A1848" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:07.895084</t>
+        </is>
+      </c>
+      <c r="B1848" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1848" t="n">
+        <v>1026.37</v>
+      </c>
+      <c r="D1848" t="n">
+        <v>2192</v>
+      </c>
+      <c r="E1848" t="n">
+        <v>73.62</v>
+      </c>
+    </row>
+    <row r="1849">
+      <c r="A1849" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:09.341554</t>
+        </is>
+      </c>
+      <c r="B1849" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1849" t="n">
+        <v>850.4299999999999</v>
+      </c>
+      <c r="D1849" t="n">
+        <v>2196.75</v>
+      </c>
+      <c r="E1849" t="n">
+        <v>82.45</v>
+      </c>
+    </row>
+    <row r="1850">
+      <c r="A1850" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:10.762119</t>
+        </is>
+      </c>
+      <c r="B1850" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1850" t="n">
+        <v>1162.63</v>
+      </c>
+      <c r="D1850" t="n">
+        <v>2105.38</v>
+      </c>
+      <c r="E1850" t="n">
+        <v>88.95</v>
+      </c>
+    </row>
+    <row r="1851">
+      <c r="A1851" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:11.899617</t>
+        </is>
+      </c>
+      <c r="B1851" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1851" t="n">
+        <v>857.0700000000001</v>
+      </c>
+      <c r="D1851" t="n">
+        <v>2072.24</v>
+      </c>
+      <c r="E1851" t="n">
+        <v>67.2</v>
+      </c>
+    </row>
+    <row r="1852">
+      <c r="A1852" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:13.024654</t>
+        </is>
+      </c>
+      <c r="B1852" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1852" t="n">
+        <v>1127.31</v>
+      </c>
+      <c r="D1852" t="n">
+        <v>2140.95</v>
+      </c>
+      <c r="E1852" t="n">
+        <v>79.48999999999999</v>
+      </c>
+    </row>
+    <row r="1853">
+      <c r="A1853" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:14.158638</t>
+        </is>
+      </c>
+      <c r="B1853" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1853" t="n">
+        <v>1143.74</v>
+      </c>
+      <c r="D1853" t="n">
+        <v>1831.63</v>
+      </c>
+      <c r="E1853" t="n">
+        <v>69.18000000000001</v>
+      </c>
+    </row>
+    <row r="1854">
+      <c r="A1854" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:15.278722</t>
+        </is>
+      </c>
+      <c r="B1854" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1854" t="n">
+        <v>1119.18</v>
+      </c>
+      <c r="D1854" t="n">
+        <v>2155.16</v>
+      </c>
+      <c r="E1854" t="n">
+        <v>67.79000000000001</v>
+      </c>
+    </row>
+    <row r="1855">
+      <c r="A1855" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:16.735985</t>
+        </is>
+      </c>
+      <c r="B1855" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1855" t="n">
+        <v>858.96</v>
+      </c>
+      <c r="D1855" t="n">
+        <v>1987.01</v>
+      </c>
+      <c r="E1855" t="n">
+        <v>69.44</v>
+      </c>
+    </row>
+    <row r="1856">
+      <c r="A1856" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:18.209138</t>
+        </is>
+      </c>
+      <c r="B1856" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1856" t="n">
+        <v>849.03</v>
+      </c>
+      <c r="D1856" t="n">
+        <v>2159.84</v>
+      </c>
+      <c r="E1856" t="n">
+        <v>71.73</v>
+      </c>
+    </row>
+    <row r="1857">
+      <c r="A1857" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:19.325693</t>
+        </is>
+      </c>
+      <c r="B1857" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1857" t="n">
+        <v>1174.17</v>
+      </c>
+      <c r="D1857" t="n">
+        <v>1809.11</v>
+      </c>
+      <c r="E1857" t="n">
+        <v>68.37</v>
+      </c>
+    </row>
+    <row r="1858">
+      <c r="A1858" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:20.456156</t>
+        </is>
+      </c>
+      <c r="B1858" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1858" t="n">
+        <v>1122.56</v>
+      </c>
+      <c r="D1858" t="n">
+        <v>1967.13</v>
+      </c>
+      <c r="E1858" t="n">
+        <v>72.31999999999999</v>
+      </c>
+    </row>
+    <row r="1859">
+      <c r="A1859" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:21.591650</t>
+        </is>
+      </c>
+      <c r="B1859" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1859" t="n">
+        <v>1043.33</v>
+      </c>
+      <c r="D1859" t="n">
+        <v>2137.7</v>
+      </c>
+      <c r="E1859" t="n">
+        <v>85.34999999999999</v>
+      </c>
+    </row>
+    <row r="1860">
+      <c r="A1860" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:22.724744</t>
+        </is>
+      </c>
+      <c r="B1860" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1860" t="n">
+        <v>924.22</v>
+      </c>
+      <c r="D1860" t="n">
+        <v>1829.28</v>
+      </c>
+      <c r="E1860" t="n">
+        <v>82.98</v>
+      </c>
+    </row>
+    <row r="1861">
+      <c r="A1861" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:23.858955</t>
+        </is>
+      </c>
+      <c r="B1861" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1861" t="n">
+        <v>831.23</v>
+      </c>
+      <c r="D1861" t="n">
+        <v>1861.37</v>
+      </c>
+      <c r="E1861" t="n">
+        <v>68.34</v>
+      </c>
+    </row>
+    <row r="1862">
+      <c r="A1862" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:24.991073</t>
+        </is>
+      </c>
+      <c r="B1862" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1862" t="n">
+        <v>1006.17</v>
+      </c>
+      <c r="D1862" t="n">
+        <v>1976.31</v>
+      </c>
+      <c r="E1862" t="n">
+        <v>81.90000000000001</v>
+      </c>
+    </row>
+    <row r="1863">
+      <c r="A1863" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:26.464927</t>
+        </is>
+      </c>
+      <c r="B1863" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1863" t="n">
+        <v>859.33</v>
+      </c>
+      <c r="D1863" t="n">
+        <v>2114.38</v>
+      </c>
+      <c r="E1863" t="n">
+        <v>67.81</v>
+      </c>
+    </row>
+    <row r="1864">
+      <c r="A1864" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:27.590517</t>
+        </is>
+      </c>
+      <c r="B1864" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1864" t="n">
+        <v>832.28</v>
+      </c>
+      <c r="D1864" t="n">
+        <v>1939.21</v>
+      </c>
+      <c r="E1864" t="n">
+        <v>86.13</v>
+      </c>
+    </row>
+    <row r="1865">
+      <c r="A1865" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:28.722928</t>
+        </is>
+      </c>
+      <c r="B1865" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1865" t="n">
+        <v>814.73</v>
+      </c>
+      <c r="D1865" t="n">
+        <v>2037.62</v>
+      </c>
+      <c r="E1865" t="n">
+        <v>82.77</v>
+      </c>
+    </row>
+    <row r="1866">
+      <c r="A1866" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:29.853447</t>
+        </is>
+      </c>
+      <c r="B1866" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1866" t="n">
+        <v>1092.64</v>
+      </c>
+      <c r="D1866" t="n">
+        <v>2171.2</v>
+      </c>
+      <c r="E1866" t="n">
+        <v>77.47</v>
+      </c>
+    </row>
+    <row r="1867">
+      <c r="A1867" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:30.991575</t>
+        </is>
+      </c>
+      <c r="B1867" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1867" t="n">
+        <v>1107.75</v>
+      </c>
+      <c r="D1867" t="n">
+        <v>2050.74</v>
+      </c>
+      <c r="E1867" t="n">
+        <v>79.18000000000001</v>
+      </c>
+    </row>
+    <row r="1868">
+      <c r="A1868" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:32.361242</t>
+        </is>
+      </c>
+      <c r="B1868" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1868" t="n">
+        <v>1185.45</v>
+      </c>
+      <c r="D1868" t="n">
+        <v>2055.26</v>
+      </c>
+      <c r="E1868" t="n">
+        <v>81.53</v>
+      </c>
+    </row>
+    <row r="1869">
+      <c r="A1869" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:33.778982</t>
+        </is>
+      </c>
+      <c r="B1869" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1869" t="n">
+        <v>1006.98</v>
+      </c>
+      <c r="D1869" t="n">
+        <v>1962.7</v>
+      </c>
+      <c r="E1869" t="n">
+        <v>75.84999999999999</v>
+      </c>
+    </row>
+    <row r="1870">
+      <c r="A1870" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:35.191627</t>
+        </is>
+      </c>
+      <c r="B1870" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1870" t="n">
+        <v>1065.6</v>
+      </c>
+      <c r="D1870" t="n">
+        <v>2140.67</v>
+      </c>
+      <c r="E1870" t="n">
+        <v>60.95</v>
+      </c>
+    </row>
+    <row r="1871">
+      <c r="A1871" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:36.595146</t>
+        </is>
+      </c>
+      <c r="B1871" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1871" t="n">
+        <v>809.99</v>
+      </c>
+      <c r="D1871" t="n">
+        <v>1879.99</v>
+      </c>
+      <c r="E1871" t="n">
+        <v>71.02</v>
+      </c>
+    </row>
+    <row r="1872">
+      <c r="A1872" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:38.045647</t>
+        </is>
+      </c>
+      <c r="B1872" t="inlineStr">
+        <is>
+          <t>WELL-1</t>
+        </is>
+      </c>
+      <c r="C1872" t="n">
+        <v>1031.63</v>
+      </c>
+      <c r="D1872" t="n">
+        <v>2169.68</v>
+      </c>
+      <c r="E1872" t="n">
+        <v>63.58</v>
+      </c>
+    </row>
+    <row r="1873">
+      <c r="A1873" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:39.177414</t>
+        </is>
+      </c>
+      <c r="B1873" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1873" t="n">
+        <v>809.14</v>
+      </c>
+      <c r="D1873" t="n">
+        <v>1971.53</v>
+      </c>
+      <c r="E1873" t="n">
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="1874">
+      <c r="A1874" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:40.292179</t>
+        </is>
+      </c>
+      <c r="B1874" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1874" t="n">
+        <v>1193.76</v>
+      </c>
+      <c r="D1874" t="n">
+        <v>2100.92</v>
+      </c>
+      <c r="E1874" t="n">
+        <v>65.06999999999999</v>
+      </c>
+    </row>
+    <row r="1875">
+      <c r="A1875" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:41.417243</t>
+        </is>
+      </c>
+      <c r="B1875" t="inlineStr">
+        <is>
+          <t>WELL-3</t>
+        </is>
+      </c>
+      <c r="C1875" t="n">
+        <v>892.76</v>
+      </c>
+      <c r="D1875" t="n">
+        <v>2003.44</v>
+      </c>
+      <c r="E1875" t="n">
+        <v>61.54</v>
+      </c>
+    </row>
+    <row r="1876">
+      <c r="A1876" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:42.557698</t>
+        </is>
+      </c>
+      <c r="B1876" t="inlineStr">
+        <is>
+          <t>WELL-4</t>
+        </is>
+      </c>
+      <c r="C1876" t="n">
+        <v>1125.18</v>
+      </c>
+      <c r="D1876" t="n">
+        <v>2063.53</v>
+      </c>
+      <c r="E1876" t="n">
+        <v>72.06</v>
+      </c>
+    </row>
+    <row r="1877">
+      <c r="A1877" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:43.676297</t>
+        </is>
+      </c>
+      <c r="B1877" t="inlineStr">
+        <is>
+          <t>WELL-5</t>
+        </is>
+      </c>
+      <c r="C1877" t="n">
+        <v>836.67</v>
+      </c>
+      <c r="D1877" t="n">
+        <v>2136.31</v>
+      </c>
+      <c r="E1877" t="n">
+        <v>88.34</v>
+      </c>
+    </row>
+    <row r="1878">
+      <c r="A1878" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:44.793950</t>
+        </is>
+      </c>
+      <c r="B1878" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1878" t="n">
+        <v>937.65</v>
+      </c>
+      <c r="D1878" t="n">
+        <v>1998.77</v>
+      </c>
+      <c r="E1878" t="n">
+        <v>72.40000000000001</v>
+      </c>
+    </row>
+    <row r="1879">
+      <c r="A1879" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:45.975264</t>
+        </is>
+      </c>
+      <c r="B1879" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1879" t="n">
+        <v>1195.04</v>
+      </c>
+      <c r="D1879" t="n">
+        <v>2047.93</v>
+      </c>
+      <c r="E1879" t="n">
+        <v>81.23</v>
+      </c>
+    </row>
+    <row r="1880">
+      <c r="A1880" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:47.122943</t>
+        </is>
+      </c>
+      <c r="B1880" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1880" t="n">
+        <v>963.09</v>
+      </c>
+      <c r="D1880" t="n">
+        <v>1988.48</v>
+      </c>
+      <c r="E1880" t="n">
+        <v>82.44</v>
+      </c>
+    </row>
+    <row r="1881">
+      <c r="A1881" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:54:48.241094</t>
+        </is>
+      </c>
+      <c r="B1881" t="inlineStr">
+        <is>
+          <t>WELL-2</t>
+        </is>
+      </c>
+      <c r="C1881" t="n">
+        <v>1165.32</v>
+      </c>
+      <c r="D1881" t="n">
+        <v>1986.09</v>
+      </c>
+      <c r="E1881" t="n">
+        <v>65.70999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>